<commit_message>
Contains LIVEHTA-67, 290, 517 regression scenarios
</commit_message>
<xml_diff>
--- a/Testdata/ImportPublicationsPage_Data_Testing.xlsx
+++ b/Testdata/ImportPublicationsPage_Data_Testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDF69E9-0C30-4152-A3E6-0C0719A6A301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAC0E49-8ADB-47E3-9AB7-7B9C519A3C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Expected_File_names</t>
   </si>
@@ -46,15 +46,9 @@
     <t>ICER RRMM - Success Case Sheet.xlsx</t>
   </si>
   <si>
-    <t>\Testdata\Templates\ImportPublications\ICER RRMM - Success Case Sheet.xlsx</t>
-  </si>
-  <si>
     <t>mCRPC - Failure Case Sheet.xlsx</t>
   </si>
   <si>
-    <t>\Testdata\Templates\ImportPublications\mCRPC - Failure Case Sheet.xlsx</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -71,16 +65,64 @@
   </si>
   <si>
     <t>IC AML - Pfizer - Ovid search - 5/10/2021</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Success Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\mCRPC - Failure Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>pop3</t>
+  </si>
+  <si>
+    <t>pop4</t>
+  </si>
+  <si>
+    <t>pop5</t>
+  </si>
+  <si>
+    <t>pop6</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Header Mismatch.xlsx</t>
+  </si>
+  <si>
+    <t>ICER RRMM - Header Mismatch.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Letters in Publication Identifier.xlsx</t>
+  </si>
+  <si>
+    <t>ICER RRMM - Letters in Publication Identifier.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Empty value in Publication Identifier.xlsx</t>
+  </si>
+  <si>
+    <t>ICER RRMM - Empty value in Publication Identifier.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Duplicate value in FA18 column.xlsx</t>
+  </si>
+  <si>
+    <t>ICER RRMM - Duplicate value in FA18 column.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,27 +434,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="2"/>
-    <col min="3" max="3" width="27.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="24.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -423,33 +465,90 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating testdata due to LIVEHTA-1904
</commit_message>
<xml_diff>
--- a/Testdata/ImportPublicationsPage_Data_Testing.xlsx
+++ b/Testdata/ImportPublicationsPage_Data_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8081CAF-965B-4C75-AB57-F2407C1CC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9E99B1-2D67-429C-945B-C19B5641501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,21 +82,12 @@
     <t>ICER RRMM - Empty value in Publication Identifier.xlsx</t>
   </si>
   <si>
-    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Duplicate value in FA18 column.xlsx</t>
-  </si>
-  <si>
-    <t>ICER RRMM - Duplicate value in FA18 column.xlsx</t>
-  </si>
-  <si>
     <t>Success Case Sheet.xlsx</t>
   </si>
   <si>
     <t>\Testdata\Templates\ImportPublications\Testing_Env\Success Case Sheet.xlsx</t>
   </si>
   <si>
-    <t>ICER - ICER RRMM 2022 report - 12/19/2022</t>
-  </si>
-  <si>
     <t>error_msg_col1</t>
   </si>
   <si>
@@ -131,6 +122,15 @@
   </si>
   <si>
     <t>There is already an existing extraction file for ICER - ICER RRMM 2022 report , please remove the previous upload and re-upload.</t>
+  </si>
+  <si>
+    <t>ICER RRMM - Duplicate value in FA19 column.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\ImportPublications\Testing_Env\ICER RRMM - Duplicate value in FA19 column.xlsx</t>
+  </si>
+  <si>
+    <t>ICER - ICER RRMM 2022 report</t>
   </si>
 </sst>
 </file>
@@ -459,14 +459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -487,13 +487,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -501,16 +501,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -518,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -530,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -560,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -614,7 +614,7 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -636,7 +636,7 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -644,19 +644,19 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -667,7 +667,7 @@
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>